<commit_message>
Target code with infix to postfix correct for dst and db examples, to be added handling negative values.
</commit_message>
<xml_diff>
--- a/Zadanie2/Zadanie2.xlsx
+++ b/Zadanie2/Zadanie2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tomek\WSM school\Paradygmaty\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tomek\WSM school\Paradygmaty\wsm_paradygmaty\Zadanie2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF85D064-905C-4BD5-BACD-55FE6B15A3ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D6DC35B-9275-42C1-986F-DBC777857196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295" xr2:uid="{2BE5AD6E-AF5D-4C4C-8940-11E2EEC7782B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2BE5AD6E-AF5D-4C4C-8940-11E2EEC7782B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="40">
   <si>
     <t>2*2-3*4+2-3*3</t>
   </si>
@@ -126,13 +126,34 @@
     <t>112 2 * 3 - 4 2 3 - + * 3 *</t>
   </si>
   <si>
-    <t>2 2 * - 3 4 * - 2 + 3 3 * -</t>
-  </si>
-  <si>
-    <t>122 21 * 13 14 * - 21 + 3 3 - * -</t>
-  </si>
-  <si>
-    <t>2 - 2 ^ 2 * 3 4 * - 2 + 3 3 - ^ -</t>
+    <t>Test Postfix</t>
+  </si>
+  <si>
+    <t>TAK</t>
+  </si>
+  <si>
+    <t>0 2 - 2 * 3 4 * - 2 + 3 3 * -</t>
+  </si>
+  <si>
+    <t>122 21 * 13 14 * - 21 + 3 0 3 - * -</t>
+  </si>
+  <si>
+    <t>0 2 - 2 ^ 2 * 3 4 * - 2 + 3 0 3 - ^ -</t>
+  </si>
+  <si>
+    <t>To do list</t>
+  </si>
+  <si>
+    <t>1.</t>
+  </si>
+  <si>
+    <t>Poprawić obsługę liczb ujemnych (przypadek na początku wprowadzonego kodu, w przypadku minusa po nawiasie lub bezpośrednio jako następstwo po innym znaku</t>
+  </si>
+  <si>
+    <t>2.</t>
+  </si>
+  <si>
+    <t>Konwersja RPN na wynik</t>
   </si>
 </sst>
 </file>
@@ -171,10 +192,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -489,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB86E75E-D202-4346-B840-956085238D1C}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A8" sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,14 +524,14 @@
     <col min="4" max="4" width="26.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -523,8 +544,11 @@
       <c r="D2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -538,8 +562,11 @@
       <c r="D3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <f>A3+1</f>
         <v>2</v>
@@ -554,8 +581,11 @@
       <c r="D4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" ref="A5:A7" si="0">A4+1</f>
         <v>3</v>
@@ -570,8 +600,11 @@
       <c r="D5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -586,8 +619,11 @@
       <c r="D6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -602,15 +638,18 @@
       <c r="D7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="E7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -621,7 +660,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -635,8 +674,11 @@
       <c r="D10" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <f>A10+1</f>
         <v>2</v>
@@ -651,8 +693,11 @@
       <c r="D11" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" ref="A12:A14" si="1">A11+1</f>
         <v>3</v>
@@ -667,8 +712,11 @@
       <c r="D12" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="1"/>
         <v>4</v>
@@ -683,8 +731,11 @@
       <c r="D13" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -699,15 +750,18 @@
       <c r="D14" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="E14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -722,7 +776,7 @@
       <c r="A17">
         <v>1</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C17">
@@ -730,7 +784,7 @@
         <v>-23</v>
       </c>
       <c r="D17" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -746,7 +800,7 @@
         <v>2410</v>
       </c>
       <c r="D18" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -754,7 +808,7 @@
         <f t="shared" ref="A19" si="2">A18+1</f>
         <v>3</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C19">
@@ -762,7 +816,28 @@
         <v>-2.0370370370370372</v>
       </c>
       <c r="D19" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added handling negative numbers at the beginning
</commit_message>
<xml_diff>
--- a/Zadanie2/Zadanie2.xlsx
+++ b/Zadanie2/Zadanie2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tomek\WSM school\Paradygmaty\wsm_paradygmaty\Zadanie2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D6DC35B-9275-42C1-986F-DBC777857196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F3D038-8344-4D5B-86EC-22ED8EE55941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2BE5AD6E-AF5D-4C4C-8940-11E2EEC7782B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
   <si>
     <t>2*2-3*4+2-3*3</t>
   </si>
@@ -513,7 +513,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A8" sqref="A1:E19"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,7 +521,7 @@
     <col min="1" max="1" width="3.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -772,7 +772,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1</v>
       </c>
@@ -786,8 +786,11 @@
       <c r="D17" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <f>A17+1</f>
         <v>2</v>
@@ -803,7 +806,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" ref="A19" si="2">A18+1</f>
         <v>3</v>
@@ -819,12 +822,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -832,7 +835,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>38</v>
       </c>

</xml_diff>

<commit_message>
program is returning the string written in Postfix and handling the negative numbers.
</commit_message>
<xml_diff>
--- a/Zadanie2/Zadanie2.xlsx
+++ b/Zadanie2/Zadanie2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tomek\WSM school\Paradygmaty\wsm_paradygmaty\Zadanie2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F3D038-8344-4D5B-86EC-22ED8EE55941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21AD1669-68C2-409E-975D-D021432D8F8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2BE5AD6E-AF5D-4C4C-8940-11E2EEC7782B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
   <si>
     <t>2*2-3*4+2-3*3</t>
   </si>
@@ -147,13 +147,13 @@
     <t>1.</t>
   </si>
   <si>
-    <t>Poprawić obsługę liczb ujemnych (przypadek na początku wprowadzonego kodu, w przypadku minusa po nawiasie lub bezpośrednio jako następstwo po innym znaku</t>
-  </si>
-  <si>
     <t>2.</t>
   </si>
   <si>
     <t>Konwersja RPN na wynik</t>
+  </si>
+  <si>
+    <t>Dodanie ekranu startowego i wyjścia, żeby można było kilkukrotnie wpisać sobie jakieś wyniki</t>
   </si>
 </sst>
 </file>
@@ -170,12 +170,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -190,12 +196,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -512,8 +519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB86E75E-D202-4346-B840-956085238D1C}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,7 +569,7 @@
       <c r="D3" t="s">
         <v>20</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="3" t="s">
         <v>31</v>
       </c>
     </row>
@@ -581,7 +588,7 @@
       <c r="D4" t="s">
         <v>21</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="3" t="s">
         <v>31</v>
       </c>
     </row>
@@ -600,7 +607,7 @@
       <c r="D5" t="s">
         <v>22</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="3" t="s">
         <v>31</v>
       </c>
     </row>
@@ -619,7 +626,7 @@
       <c r="D6" t="s">
         <v>23</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="3" t="s">
         <v>31</v>
       </c>
     </row>
@@ -638,7 +645,7 @@
       <c r="D7" t="s">
         <v>24</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="3" t="s">
         <v>31</v>
       </c>
     </row>
@@ -674,7 +681,7 @@
       <c r="D10" t="s">
         <v>25</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="3" t="s">
         <v>31</v>
       </c>
     </row>
@@ -693,7 +700,7 @@
       <c r="D11" t="s">
         <v>26</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="3" t="s">
         <v>31</v>
       </c>
     </row>
@@ -712,7 +719,7 @@
       <c r="D12" t="s">
         <v>27</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="3" t="s">
         <v>31</v>
       </c>
     </row>
@@ -731,7 +738,7 @@
       <c r="D13" t="s">
         <v>28</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="3" t="s">
         <v>31</v>
       </c>
     </row>
@@ -750,7 +757,7 @@
       <c r="D14" t="s">
         <v>29</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="3" t="s">
         <v>31</v>
       </c>
     </row>
@@ -786,7 +793,7 @@
       <c r="D17" t="s">
         <v>32</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="3" t="s">
         <v>31</v>
       </c>
     </row>
@@ -805,6 +812,9 @@
       <c r="D18" t="s">
         <v>33</v>
       </c>
+      <c r="E18" s="3" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
@@ -821,6 +831,9 @@
       <c r="D19" t="s">
         <v>34</v>
       </c>
+      <c r="E19" s="3" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -832,12 +845,12 @@
         <v>36</v>
       </c>
       <c r="B23" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B24" t="s">
         <v>39</v>

</xml_diff>